<commit_message>
Added SupTab3 column descriptions and fixed typos
</commit_message>
<xml_diff>
--- a/SupplementalMaterial/S2_Dawson_PFAS_HL_102422.xlsx
+++ b/SupplementalMaterial/S2_Dawson_PFAS_HL_102422.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\CompTox-PFASHalfLife\SupplementalMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F2CD63-1086-4F5D-A8D2-9C9ACB8058D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEDF1404-4552-437C-9976-6A60134F6DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="896" xr2:uid="{3AE89EC0-E899-4B86-9873-BFB640045260}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="896" xr2:uid="{3AE89EC0-E899-4B86-9873-BFB640045260}"/>
   </bookViews>
   <sheets>
     <sheet name="S2.0_Index" sheetId="12" r:id="rId1"/>
@@ -934,9 +934,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>PFAS Half-life data from liturature sources used to derive the training set</t>
-  </si>
-  <si>
     <t>Chemical structures of all training set chemicals</t>
   </si>
   <si>
@@ -1694,6 +1691,9 @@
   </si>
   <si>
     <t>S2.6</t>
+  </si>
+  <si>
+    <t>PFAS Half-life data from literature sources used to derive the training set</t>
   </si>
 </sst>
 </file>
@@ -2425,16 +2425,97 @@
     <xf numFmtId="164" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2445,73 +2526,10 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2540,24 +2558,6 @@
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4165,8 +4165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D73D269-8AB1-4513-832B-8835F17F51A6}">
   <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:G14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4177,19 +4177,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="111" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="110" t="s">
-        <v>474</v>
-      </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
-      <c r="G1" s="110"/>
-      <c r="H1" s="110"/>
-      <c r="I1" s="110"/>
-      <c r="J1" s="110"/>
-      <c r="K1" s="110"/>
+      <c r="A1" s="116" t="s">
+        <v>473</v>
+      </c>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
+      <c r="I1" s="116"/>
+      <c r="J1" s="116"/>
+      <c r="K1" s="116"/>
       <c r="L1" s="38"/>
       <c r="M1" s="38"/>
       <c r="N1" s="38"/>
@@ -4199,19 +4199,19 @@
       <c r="R1" s="38"/>
     </row>
     <row r="2" spans="1:18" ht="37.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="111" t="s">
-        <v>475</v>
-      </c>
-      <c r="B2" s="111"/>
-      <c r="C2" s="111"/>
-      <c r="D2" s="111"/>
-      <c r="E2" s="111"/>
-      <c r="F2" s="111"/>
-      <c r="G2" s="111"/>
-      <c r="H2" s="111"/>
-      <c r="I2" s="111"/>
-      <c r="J2" s="111"/>
-      <c r="K2" s="111"/>
+      <c r="A2" s="117" t="s">
+        <v>474</v>
+      </c>
+      <c r="B2" s="117"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="117"/>
       <c r="L2" s="37"/>
       <c r="M2" s="37"/>
       <c r="N2" s="37"/>
@@ -4221,19 +4221,19 @@
       <c r="R2" s="37"/>
     </row>
     <row r="3" spans="1:18" ht="109.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="111" t="s">
+      <c r="A3" s="117" t="s">
         <v>292</v>
       </c>
-      <c r="B3" s="111"/>
-      <c r="C3" s="111"/>
-      <c r="D3" s="111"/>
-      <c r="E3" s="111"/>
-      <c r="F3" s="111"/>
-      <c r="G3" s="111"/>
-      <c r="H3" s="111"/>
-      <c r="I3" s="111"/>
-      <c r="J3" s="111"/>
-      <c r="K3" s="111"/>
+      <c r="B3" s="117"/>
+      <c r="C3" s="117"/>
+      <c r="D3" s="117"/>
+      <c r="E3" s="117"/>
+      <c r="F3" s="117"/>
+      <c r="G3" s="117"/>
+      <c r="H3" s="117"/>
+      <c r="I3" s="117"/>
+      <c r="J3" s="117"/>
+      <c r="K3" s="117"/>
       <c r="L3" s="37"/>
       <c r="M3" s="37"/>
       <c r="N3" s="37"/>
@@ -4259,121 +4259,121 @@
       <c r="G5" s="39"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A6" s="150" t="s">
+      <c r="A6" s="110" t="s">
+        <v>475</v>
+      </c>
+      <c r="B6" s="114" t="s">
+        <v>482</v>
+      </c>
+      <c r="C6" s="114"/>
+      <c r="D6" s="114"/>
+      <c r="E6" s="114"/>
+      <c r="F6" s="114"/>
+      <c r="G6" s="114"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A7" s="110" t="s">
         <v>476</v>
       </c>
-      <c r="B6" s="151" t="s">
+      <c r="B7" s="111" t="s">
+        <v>477</v>
+      </c>
+      <c r="C7" s="111"/>
+      <c r="D7" s="111"/>
+      <c r="E7" s="111"/>
+      <c r="F7" s="111"/>
+      <c r="G7" s="111"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A8" s="110" t="s">
+        <v>431</v>
+      </c>
+      <c r="B8" s="111" t="s">
+        <v>432</v>
+      </c>
+      <c r="C8" s="111"/>
+      <c r="D8" s="111"/>
+      <c r="E8" s="111"/>
+      <c r="F8" s="111"/>
+      <c r="G8" s="111"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A9" s="112" t="s">
+        <v>478</v>
+      </c>
+      <c r="B9" s="111" t="s">
         <v>295</v>
       </c>
-      <c r="C6" s="151"/>
-      <c r="D6" s="151"/>
-      <c r="E6" s="151"/>
-      <c r="F6" s="151"/>
-      <c r="G6" s="151"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A7" s="150" t="s">
-        <v>477</v>
-      </c>
-      <c r="B7" s="152" t="s">
-        <v>478</v>
-      </c>
-      <c r="C7" s="152"/>
-      <c r="D7" s="152"/>
-      <c r="E7" s="152"/>
-      <c r="F7" s="152"/>
-      <c r="G7" s="152"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A8" s="150" t="s">
-        <v>432</v>
-      </c>
-      <c r="B8" s="152" t="s">
+      <c r="C9" s="111"/>
+      <c r="D9" s="111"/>
+      <c r="E9" s="111"/>
+      <c r="F9" s="111"/>
+      <c r="G9" s="111"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A10" s="112" t="s">
+        <v>479</v>
+      </c>
+      <c r="B10" s="111" t="s">
+        <v>296</v>
+      </c>
+      <c r="C10" s="111"/>
+      <c r="D10" s="111"/>
+      <c r="E10" s="111"/>
+      <c r="F10" s="111"/>
+      <c r="G10" s="111"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A11" s="112" t="s">
+        <v>429</v>
+      </c>
+      <c r="B11" s="111" t="s">
         <v>433</v>
       </c>
-      <c r="C8" s="152"/>
-      <c r="D8" s="152"/>
-      <c r="E8" s="152"/>
-      <c r="F8" s="152"/>
-      <c r="G8" s="152"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A9" s="153" t="s">
-        <v>479</v>
-      </c>
-      <c r="B9" s="152" t="s">
-        <v>296</v>
-      </c>
-      <c r="C9" s="152"/>
-      <c r="D9" s="152"/>
-      <c r="E9" s="152"/>
-      <c r="F9" s="152"/>
-      <c r="G9" s="152"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A10" s="153" t="s">
+      <c r="C11" s="111"/>
+      <c r="D11" s="111"/>
+      <c r="E11" s="111"/>
+      <c r="F11" s="111"/>
+      <c r="G11" s="111"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A12" s="112" t="s">
+        <v>418</v>
+      </c>
+      <c r="B12" t="s">
+        <v>430</v>
+      </c>
+      <c r="C12" s="111"/>
+      <c r="D12" s="111"/>
+      <c r="E12" s="111"/>
+      <c r="F12" s="111"/>
+      <c r="G12" s="111"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A13" s="112" t="s">
         <v>480</v>
       </c>
-      <c r="B10" s="152" t="s">
+      <c r="B13" s="111" t="s">
         <v>297</v>
       </c>
-      <c r="C10" s="152"/>
-      <c r="D10" s="152"/>
-      <c r="E10" s="152"/>
-      <c r="F10" s="152"/>
-      <c r="G10" s="152"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A11" s="153" t="s">
-        <v>430</v>
-      </c>
-      <c r="B11" s="152" t="s">
-        <v>434</v>
-      </c>
-      <c r="C11" s="152"/>
-      <c r="D11" s="152"/>
-      <c r="E11" s="152"/>
-      <c r="F11" s="152"/>
-      <c r="G11" s="152"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A12" s="153" t="s">
-        <v>419</v>
-      </c>
-      <c r="B12" t="s">
-        <v>431</v>
-      </c>
-      <c r="C12" s="152"/>
-      <c r="D12" s="152"/>
-      <c r="E12" s="152"/>
-      <c r="F12" s="152"/>
-      <c r="G12" s="152"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A13" s="153" t="s">
+      <c r="C13" s="111"/>
+      <c r="D13" s="111"/>
+      <c r="E13" s="111"/>
+      <c r="F13" s="111"/>
+      <c r="G13" s="111"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A14" s="113" t="s">
         <v>481</v>
       </c>
-      <c r="B13" s="152" t="s">
+      <c r="B14" s="115" t="s">
         <v>298</v>
       </c>
-      <c r="C13" s="152"/>
-      <c r="D13" s="152"/>
-      <c r="E13" s="152"/>
-      <c r="F13" s="152"/>
-      <c r="G13" s="152"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A14" s="154" t="s">
-        <v>482</v>
-      </c>
-      <c r="B14" s="155" t="s">
-        <v>299</v>
-      </c>
-      <c r="C14" s="155"/>
-      <c r="D14" s="155"/>
-      <c r="E14" s="155"/>
-      <c r="F14" s="155"/>
-      <c r="G14" s="155"/>
+      <c r="C14" s="115"/>
+      <c r="D14" s="115"/>
+      <c r="E14" s="115"/>
+      <c r="F14" s="115"/>
+      <c r="G14" s="115"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -6289,7 +6289,7 @@
         <v>63</v>
       </c>
       <c r="N2" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O2" s="44" t="s">
         <v>59</v>
@@ -6347,7 +6347,7 @@
         <v>63</v>
       </c>
       <c r="N3" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O3" s="44" t="s">
         <v>59</v>
@@ -6407,7 +6407,7 @@
         <v>7</v>
       </c>
       <c r="N4" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O4" s="44" t="s">
         <v>57</v>
@@ -6471,7 +6471,7 @@
         <v>7</v>
       </c>
       <c r="N5" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O5" s="44" t="s">
         <v>57</v>
@@ -6527,7 +6527,7 @@
         <v>7</v>
       </c>
       <c r="N6" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O6" s="44" t="s">
         <v>54</v>
@@ -6587,7 +6587,7 @@
         <v>6</v>
       </c>
       <c r="N7" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O7" s="44" t="s">
         <v>59</v>
@@ -6645,7 +6645,7 @@
         <v>6</v>
       </c>
       <c r="N8" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O8" s="44" t="s">
         <v>59</v>
@@ -6829,7 +6829,7 @@
         <v>6</v>
       </c>
       <c r="N11" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O11" s="44" t="s">
         <v>54</v>
@@ -6891,7 +6891,7 @@
         <v>6</v>
       </c>
       <c r="N12" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O12" s="44" t="s">
         <v>54</v>
@@ -6953,7 +6953,7 @@
         <v>6</v>
       </c>
       <c r="N13" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O13" s="44" t="s">
         <v>54</v>
@@ -7015,7 +7015,7 @@
         <v>6</v>
       </c>
       <c r="N14" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O14" s="44" t="s">
         <v>54</v>
@@ -7077,7 +7077,7 @@
         <v>6</v>
       </c>
       <c r="N15" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O15" s="44" t="s">
         <v>54</v>
@@ -7139,7 +7139,7 @@
         <v>6</v>
       </c>
       <c r="N16" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O16" s="44" t="s">
         <v>54</v>
@@ -7201,7 +7201,7 @@
         <v>6</v>
       </c>
       <c r="N17" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O17" s="42" t="s">
         <v>54</v>
@@ -7261,7 +7261,7 @@
         <v>6</v>
       </c>
       <c r="N18" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O18" s="42" t="s">
         <v>54</v>
@@ -7321,7 +7321,7 @@
         <v>7</v>
       </c>
       <c r="N19" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O19" s="48" t="s">
         <v>57</v>
@@ -7383,7 +7383,7 @@
         <v>7</v>
       </c>
       <c r="N20" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O20" s="48" t="s">
         <v>57</v>
@@ -7437,7 +7437,7 @@
         <v>7</v>
       </c>
       <c r="N21" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O21" s="44" t="s">
         <v>54</v>
@@ -7491,7 +7491,7 @@
         <v>7</v>
       </c>
       <c r="N22" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O22" s="44" t="s">
         <v>54</v>
@@ -7545,7 +7545,7 @@
         <v>7</v>
       </c>
       <c r="N23" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O23" s="44" t="s">
         <v>54</v>
@@ -7599,7 +7599,7 @@
         <v>7</v>
       </c>
       <c r="N24" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O24" s="44" t="s">
         <v>54</v>
@@ -7661,7 +7661,7 @@
         <v>7</v>
       </c>
       <c r="N25" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O25" s="44" t="s">
         <v>54</v>
@@ -7723,7 +7723,7 @@
         <v>7</v>
       </c>
       <c r="N26" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O26" s="44" t="s">
         <v>54</v>
@@ -7785,7 +7785,7 @@
         <v>7</v>
       </c>
       <c r="N27" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O27" s="44" t="s">
         <v>54</v>
@@ -7847,7 +7847,7 @@
         <v>7</v>
       </c>
       <c r="N28" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O28" s="44" t="s">
         <v>54</v>
@@ -7909,7 +7909,7 @@
         <v>6</v>
       </c>
       <c r="N29" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O29" s="48" t="s">
         <v>57</v>
@@ -7973,7 +7973,7 @@
         <v>6</v>
       </c>
       <c r="N30" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O30" s="48" t="s">
         <v>57</v>
@@ -9853,7 +9853,7 @@
         <v>6</v>
       </c>
       <c r="N61" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O61" s="44" t="s">
         <v>54</v>
@@ -9977,7 +9977,7 @@
         <v>6</v>
       </c>
       <c r="N63" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O63" s="44" t="s">
         <v>54</v>
@@ -10039,7 +10039,7 @@
         <v>6</v>
       </c>
       <c r="N64" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O64" s="44" t="s">
         <v>54</v>
@@ -10322,7 +10322,7 @@
         <v>253</v>
       </c>
       <c r="C69" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D69" s="47" t="s">
         <v>4</v>
@@ -10376,7 +10376,7 @@
         <v>253</v>
       </c>
       <c r="C70" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D70" s="47" t="s">
         <v>8</v>
@@ -10430,7 +10430,7 @@
         <v>253</v>
       </c>
       <c r="C71" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D71" s="47" t="s">
         <v>4</v>
@@ -10484,7 +10484,7 @@
         <v>253</v>
       </c>
       <c r="C72" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D72" s="47" t="s">
         <v>8</v>
@@ -10538,7 +10538,7 @@
         <v>253</v>
       </c>
       <c r="C73" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D73" s="47" t="s">
         <v>4</v>
@@ -10592,7 +10592,7 @@
         <v>253</v>
       </c>
       <c r="C74" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D74" s="47" t="s">
         <v>4</v>
@@ -10646,7 +10646,7 @@
         <v>253</v>
       </c>
       <c r="C75" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D75" s="47" t="s">
         <v>8</v>
@@ -10700,7 +10700,7 @@
         <v>253</v>
       </c>
       <c r="C76" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D76" s="47" t="s">
         <v>8</v>
@@ -11681,10 +11681,10 @@
         <v>155</v>
       </c>
       <c r="B92" s="54" t="s">
+        <v>382</v>
+      </c>
+      <c r="C92" t="s">
         <v>383</v>
-      </c>
-      <c r="C92" t="s">
-        <v>384</v>
       </c>
       <c r="D92" s="45" t="s">
         <v>4</v>
@@ -11739,10 +11739,10 @@
         <v>155</v>
       </c>
       <c r="B93" s="54" t="s">
+        <v>382</v>
+      </c>
+      <c r="C93" t="s">
         <v>383</v>
-      </c>
-      <c r="C93" t="s">
-        <v>384</v>
       </c>
       <c r="D93" s="45" t="s">
         <v>4</v>
@@ -11797,10 +11797,10 @@
         <v>155</v>
       </c>
       <c r="B94" s="54" t="s">
+        <v>382</v>
+      </c>
+      <c r="C94" t="s">
         <v>383</v>
-      </c>
-      <c r="C94" t="s">
-        <v>384</v>
       </c>
       <c r="D94" s="45" t="s">
         <v>4</v>
@@ -11855,10 +11855,10 @@
         <v>155</v>
       </c>
       <c r="B95" s="54" t="s">
+        <v>382</v>
+      </c>
+      <c r="C95" t="s">
         <v>383</v>
-      </c>
-      <c r="C95" t="s">
-        <v>384</v>
       </c>
       <c r="D95" s="45" t="s">
         <v>4</v>
@@ -11913,10 +11913,10 @@
         <v>155</v>
       </c>
       <c r="B96" s="54" t="s">
+        <v>382</v>
+      </c>
+      <c r="C96" t="s">
         <v>383</v>
-      </c>
-      <c r="C96" t="s">
-        <v>384</v>
       </c>
       <c r="D96" s="45" t="s">
         <v>8</v>
@@ -11971,10 +11971,10 @@
         <v>155</v>
       </c>
       <c r="B97" s="54" t="s">
+        <v>382</v>
+      </c>
+      <c r="C97" t="s">
         <v>383</v>
-      </c>
-      <c r="C97" t="s">
-        <v>384</v>
       </c>
       <c r="D97" s="45" t="s">
         <v>8</v>
@@ -12029,10 +12029,10 @@
         <v>155</v>
       </c>
       <c r="B98" s="54" t="s">
+        <v>382</v>
+      </c>
+      <c r="C98" t="s">
         <v>383</v>
-      </c>
-      <c r="C98" t="s">
-        <v>384</v>
       </c>
       <c r="D98" s="45" t="s">
         <v>8</v>
@@ -12087,10 +12087,10 @@
         <v>155</v>
       </c>
       <c r="B99" s="54" t="s">
+        <v>382</v>
+      </c>
+      <c r="C99" t="s">
         <v>383</v>
-      </c>
-      <c r="C99" t="s">
-        <v>384</v>
       </c>
       <c r="D99" s="45" t="s">
         <v>8</v>
@@ -12175,7 +12175,7 @@
         <v>6</v>
       </c>
       <c r="N100" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O100" s="44" t="s">
         <v>126</v>
@@ -12231,7 +12231,7 @@
         <v>6</v>
       </c>
       <c r="N101" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O101" s="44" t="s">
         <v>126</v>
@@ -12287,7 +12287,7 @@
         <v>6</v>
       </c>
       <c r="N102" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O102" s="44" t="s">
         <v>126</v>
@@ -12343,7 +12343,7 @@
         <v>6</v>
       </c>
       <c r="N103" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O103" s="44" t="s">
         <v>126</v>
@@ -12399,7 +12399,7 @@
         <v>6</v>
       </c>
       <c r="N104" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O104" s="44" t="s">
         <v>126</v>
@@ -12453,7 +12453,7 @@
         <v>6</v>
       </c>
       <c r="N105" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O105" s="44" t="s">
         <v>126</v>
@@ -12477,10 +12477,10 @@
         <v>128</v>
       </c>
       <c r="B106" s="54" t="s">
+        <v>380</v>
+      </c>
+      <c r="C106" t="s">
         <v>381</v>
-      </c>
-      <c r="C106" t="s">
-        <v>382</v>
       </c>
       <c r="D106" s="47" t="s">
         <v>4</v>
@@ -12505,7 +12505,7 @@
         <v>7</v>
       </c>
       <c r="N106" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O106" s="44" t="s">
         <v>126</v>
@@ -12529,10 +12529,10 @@
         <v>128</v>
       </c>
       <c r="B107" s="54" t="s">
+        <v>380</v>
+      </c>
+      <c r="C107" t="s">
         <v>381</v>
-      </c>
-      <c r="C107" t="s">
-        <v>382</v>
       </c>
       <c r="D107" s="47" t="s">
         <v>4</v>
@@ -12557,7 +12557,7 @@
         <v>7</v>
       </c>
       <c r="N107" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O107" s="44" t="s">
         <v>126</v>
@@ -12581,10 +12581,10 @@
         <v>128</v>
       </c>
       <c r="B108" s="54" t="s">
+        <v>380</v>
+      </c>
+      <c r="C108" t="s">
         <v>381</v>
-      </c>
-      <c r="C108" t="s">
-        <v>382</v>
       </c>
       <c r="D108" s="47" t="s">
         <v>8</v>
@@ -12609,7 +12609,7 @@
         <v>7</v>
       </c>
       <c r="N108" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O108" s="44" t="s">
         <v>126</v>
@@ -12633,10 +12633,10 @@
         <v>128</v>
       </c>
       <c r="B109" s="54" t="s">
+        <v>380</v>
+      </c>
+      <c r="C109" t="s">
         <v>381</v>
-      </c>
-      <c r="C109" t="s">
-        <v>382</v>
       </c>
       <c r="D109" s="47" t="s">
         <v>8</v>
@@ -12661,7 +12661,7 @@
         <v>7</v>
       </c>
       <c r="N109" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O109" s="44" t="s">
         <v>126</v>
@@ -12685,10 +12685,10 @@
         <v>128</v>
       </c>
       <c r="B110" s="54" t="s">
+        <v>380</v>
+      </c>
+      <c r="C110" t="s">
         <v>381</v>
-      </c>
-      <c r="C110" t="s">
-        <v>382</v>
       </c>
       <c r="D110" s="47" t="s">
         <v>8</v>
@@ -12713,7 +12713,7 @@
         <v>7</v>
       </c>
       <c r="N110" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O110" s="44" t="s">
         <v>126</v>
@@ -13015,7 +13015,7 @@
         <v>7</v>
       </c>
       <c r="N115" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O115" s="44" t="s">
         <v>54</v>
@@ -13075,7 +13075,7 @@
         <v>7</v>
       </c>
       <c r="N116" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O116" s="44" t="s">
         <v>57</v>
@@ -13135,7 +13135,7 @@
         <v>7</v>
       </c>
       <c r="N117" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O117" s="44" t="s">
         <v>57</v>
@@ -13195,7 +13195,7 @@
         <v>7</v>
       </c>
       <c r="N118" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O118" s="44" t="s">
         <v>54</v>
@@ -13495,7 +13495,7 @@
         <v>7</v>
       </c>
       <c r="N123" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O123" s="44" t="s">
         <v>57</v>
@@ -13559,7 +13559,7 @@
         <v>7</v>
       </c>
       <c r="N124" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O124" s="44" t="s">
         <v>54</v>
@@ -13623,7 +13623,7 @@
         <v>7</v>
       </c>
       <c r="N125" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O125" s="44" t="s">
         <v>54</v>
@@ -13687,7 +13687,7 @@
         <v>7</v>
       </c>
       <c r="N126" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O126" s="44" t="s">
         <v>57</v>
@@ -14005,7 +14005,7 @@
         <v>6</v>
       </c>
       <c r="N131" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O131" s="44" t="s">
         <v>54</v>
@@ -14065,7 +14065,7 @@
         <v>6</v>
       </c>
       <c r="N132" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O132" s="44" t="s">
         <v>54</v>
@@ -14125,7 +14125,7 @@
         <v>63</v>
       </c>
       <c r="N133" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O133" s="44" t="s">
         <v>59</v>
@@ -14185,7 +14185,7 @@
         <v>63</v>
       </c>
       <c r="N134" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O134" s="44" t="s">
         <v>59</v>
@@ -14245,7 +14245,7 @@
         <v>63</v>
       </c>
       <c r="N135" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O135" s="44" t="s">
         <v>59</v>
@@ -14305,7 +14305,7 @@
         <v>63</v>
       </c>
       <c r="N136" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O136" s="44" t="s">
         <v>59</v>
@@ -14365,7 +14365,7 @@
         <v>63</v>
       </c>
       <c r="N137" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O137" s="44" t="s">
         <v>59</v>
@@ -14423,7 +14423,7 @@
         <v>63</v>
       </c>
       <c r="N138" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O138" s="44" t="s">
         <v>59</v>
@@ -14483,7 +14483,7 @@
         <v>63</v>
       </c>
       <c r="N139" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O139" s="44" t="s">
         <v>59</v>
@@ -14543,7 +14543,7 @@
         <v>63</v>
       </c>
       <c r="N140" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O140" s="44" t="s">
         <v>59</v>
@@ -14601,7 +14601,7 @@
         <v>63</v>
       </c>
       <c r="N141" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O141" s="44" t="s">
         <v>59</v>
@@ -14661,7 +14661,7 @@
         <v>63</v>
       </c>
       <c r="N142" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O142" s="44" t="s">
         <v>59</v>
@@ -14721,7 +14721,7 @@
         <v>7</v>
       </c>
       <c r="N143" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O143" s="42" t="s">
         <v>54</v>
@@ -14781,7 +14781,7 @@
         <v>7</v>
       </c>
       <c r="N144" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O144" s="42" t="s">
         <v>54</v>
@@ -14843,7 +14843,7 @@
         <v>7</v>
       </c>
       <c r="N145" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O145" s="44" t="s">
         <v>54</v>
@@ -14907,7 +14907,7 @@
         <v>7</v>
       </c>
       <c r="N146" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O146" s="44" t="s">
         <v>54</v>
@@ -14971,7 +14971,7 @@
         <v>7</v>
       </c>
       <c r="N147" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O147" s="44" t="s">
         <v>57</v>
@@ -15035,7 +15035,7 @@
         <v>7</v>
       </c>
       <c r="N148" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O148" s="44" t="s">
         <v>57</v>
@@ -15099,7 +15099,7 @@
         <v>7</v>
       </c>
       <c r="N149" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O149" s="44" t="s">
         <v>57</v>
@@ -15163,7 +15163,7 @@
         <v>7</v>
       </c>
       <c r="N150" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O150" s="44" t="s">
         <v>57</v>
@@ -15227,7 +15227,7 @@
         <v>7</v>
       </c>
       <c r="N151" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O151" s="44" t="s">
         <v>57</v>
@@ -15289,7 +15289,7 @@
         <v>7</v>
       </c>
       <c r="N152" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O152" s="44" t="s">
         <v>57</v>
@@ -15349,7 +15349,7 @@
         <v>63</v>
       </c>
       <c r="N153" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O153" s="44" t="s">
         <v>59</v>
@@ -15407,7 +15407,7 @@
         <v>63</v>
       </c>
       <c r="N154" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O154" s="44" t="s">
         <v>59</v>
@@ -15465,7 +15465,7 @@
         <v>63</v>
       </c>
       <c r="N155" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O155" s="44" t="s">
         <v>59</v>
@@ -15523,7 +15523,7 @@
         <v>63</v>
       </c>
       <c r="N156" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O156" s="44" t="s">
         <v>59</v>
@@ -15581,7 +15581,7 @@
         <v>7</v>
       </c>
       <c r="N157" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O157" s="44" t="s">
         <v>59</v>
@@ -15639,7 +15639,7 @@
         <v>7</v>
       </c>
       <c r="N158" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O158" s="44" t="s">
         <v>59</v>
@@ -15941,7 +15941,7 @@
         <v>7</v>
       </c>
       <c r="N163" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O163" s="44" t="s">
         <v>59</v>
@@ -15999,7 +15999,7 @@
         <v>7</v>
       </c>
       <c r="N164" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O164" s="44" t="s">
         <v>59</v>
@@ -16021,10 +16021,10 @@
         <v>42</v>
       </c>
       <c r="B165" s="54" t="s">
+        <v>384</v>
+      </c>
+      <c r="C165" t="s">
         <v>385</v>
-      </c>
-      <c r="C165" t="s">
-        <v>386</v>
       </c>
       <c r="D165" s="45" t="s">
         <v>4</v>
@@ -16057,7 +16057,7 @@
         <v>63</v>
       </c>
       <c r="N165" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O165" s="44" t="s">
         <v>59</v>
@@ -16081,10 +16081,10 @@
         <v>42</v>
       </c>
       <c r="B166" s="54" t="s">
+        <v>384</v>
+      </c>
+      <c r="C166" t="s">
         <v>385</v>
-      </c>
-      <c r="C166" t="s">
-        <v>386</v>
       </c>
       <c r="D166" s="45" t="s">
         <v>8</v>
@@ -16117,7 +16117,7 @@
         <v>63</v>
       </c>
       <c r="N166" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O166" s="44" t="s">
         <v>59</v>
@@ -16179,7 +16179,7 @@
         <v>7</v>
       </c>
       <c r="N167" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O167" s="48" t="s">
         <v>57</v>
@@ -16241,7 +16241,7 @@
         <v>7</v>
       </c>
       <c r="N168" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O168" s="48" t="s">
         <v>57</v>
@@ -16295,7 +16295,7 @@
         <v>7</v>
       </c>
       <c r="N169" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O169" s="44" t="s">
         <v>54</v>
@@ -16349,7 +16349,7 @@
         <v>7</v>
       </c>
       <c r="N170" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O170" s="44" t="s">
         <v>54</v>
@@ -16403,7 +16403,7 @@
         <v>7</v>
       </c>
       <c r="N171" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O171" s="44" t="s">
         <v>54</v>
@@ -16457,7 +16457,7 @@
         <v>7</v>
       </c>
       <c r="N172" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O172" s="44" t="s">
         <v>54</v>
@@ -17231,7 +17231,7 @@
         <v>7</v>
       </c>
       <c r="N185" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O185" s="44" t="s">
         <v>57</v>
@@ -17285,7 +17285,7 @@
         <v>7</v>
       </c>
       <c r="N186" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O186" s="44" t="s">
         <v>57</v>
@@ -17345,7 +17345,7 @@
         <v>63</v>
       </c>
       <c r="N187" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O187" s="44" t="s">
         <v>59</v>
@@ -17405,7 +17405,7 @@
         <v>63</v>
       </c>
       <c r="N188" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O188" s="44" t="s">
         <v>59</v>
@@ -17465,7 +17465,7 @@
         <v>63</v>
       </c>
       <c r="N189" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O189" s="44" t="s">
         <v>59</v>
@@ -17525,7 +17525,7 @@
         <v>63</v>
       </c>
       <c r="N190" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O190" s="44" t="s">
         <v>59</v>
@@ -17585,7 +17585,7 @@
         <v>63</v>
       </c>
       <c r="N191" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O191" s="44" t="s">
         <v>59</v>
@@ -17645,7 +17645,7 @@
         <v>63</v>
       </c>
       <c r="N192" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O192" s="44" t="s">
         <v>59</v>
@@ -17705,7 +17705,7 @@
         <v>63</v>
       </c>
       <c r="N193" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O193" s="44" t="s">
         <v>59</v>
@@ -17765,7 +17765,7 @@
         <v>63</v>
       </c>
       <c r="N194" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O194" s="44" t="s">
         <v>59</v>
@@ -17823,7 +17823,7 @@
         <v>63</v>
       </c>
       <c r="N195" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O195" s="44" t="s">
         <v>59</v>
@@ -17881,7 +17881,7 @@
         <v>63</v>
       </c>
       <c r="N196" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O196" s="44" t="s">
         <v>59</v>
@@ -17941,7 +17941,7 @@
         <v>63</v>
       </c>
       <c r="N197" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O197" s="44" t="s">
         <v>59</v>
@@ -18001,7 +18001,7 @@
         <v>63</v>
       </c>
       <c r="N198" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O198" s="44" t="s">
         <v>59</v>
@@ -18061,7 +18061,7 @@
         <v>63</v>
       </c>
       <c r="N199" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O199" s="44" t="s">
         <v>59</v>
@@ -18121,7 +18121,7 @@
         <v>63</v>
       </c>
       <c r="N200" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O200" s="44" t="s">
         <v>59</v>
@@ -18181,7 +18181,7 @@
         <v>63</v>
       </c>
       <c r="N201" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O201" s="44" t="s">
         <v>59</v>
@@ -18241,7 +18241,7 @@
         <v>63</v>
       </c>
       <c r="N202" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O202" s="44" t="s">
         <v>59</v>
@@ -18265,10 +18265,10 @@
         <v>65</v>
       </c>
       <c r="B203" s="54" t="s">
+        <v>387</v>
+      </c>
+      <c r="C203" t="s">
         <v>388</v>
-      </c>
-      <c r="C203" t="s">
-        <v>389</v>
       </c>
       <c r="D203" s="45" t="s">
         <v>4</v>
@@ -18299,7 +18299,7 @@
         <v>63</v>
       </c>
       <c r="N203" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O203" s="44" t="s">
         <v>59</v>
@@ -18323,10 +18323,10 @@
         <v>65</v>
       </c>
       <c r="B204" s="54" t="s">
+        <v>387</v>
+      </c>
+      <c r="C204" t="s">
         <v>388</v>
-      </c>
-      <c r="C204" t="s">
-        <v>389</v>
       </c>
       <c r="D204" s="45" t="s">
         <v>8</v>
@@ -18357,7 +18357,7 @@
         <v>63</v>
       </c>
       <c r="N204" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O204" s="44" t="s">
         <v>59</v>
@@ -18415,7 +18415,7 @@
         <v>63</v>
       </c>
       <c r="N205" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O205" s="44" t="s">
         <v>59</v>
@@ -18473,7 +18473,7 @@
         <v>63</v>
       </c>
       <c r="N206" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O206" s="44" t="s">
         <v>59</v>
@@ -18531,7 +18531,7 @@
         <v>63</v>
       </c>
       <c r="N207" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O207" s="44" t="s">
         <v>59</v>
@@ -18589,7 +18589,7 @@
         <v>63</v>
       </c>
       <c r="N208" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O208" s="44" t="s">
         <v>59</v>
@@ -18649,7 +18649,7 @@
         <v>63</v>
       </c>
       <c r="N209" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O209" s="44" t="s">
         <v>59</v>
@@ -18709,7 +18709,7 @@
         <v>63</v>
       </c>
       <c r="N210" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O210" s="44" t="s">
         <v>59</v>
@@ -18769,7 +18769,7 @@
         <v>63</v>
       </c>
       <c r="N211" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O211" s="44" t="s">
         <v>59</v>
@@ -18829,7 +18829,7 @@
         <v>63</v>
       </c>
       <c r="N212" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O212" s="44" t="s">
         <v>59</v>
@@ -18889,7 +18889,7 @@
         <v>63</v>
       </c>
       <c r="N213" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O213" s="44" t="s">
         <v>59</v>
@@ -18949,7 +18949,7 @@
         <v>63</v>
       </c>
       <c r="N214" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O214" s="44" t="s">
         <v>59</v>
@@ -19009,7 +19009,7 @@
         <v>63</v>
       </c>
       <c r="N215" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O215" s="44" t="s">
         <v>59</v>
@@ -19069,7 +19069,7 @@
         <v>63</v>
       </c>
       <c r="N216" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O216" s="44" t="s">
         <v>59</v>
@@ -19697,10 +19697,10 @@
         <v>217</v>
       </c>
       <c r="M1" t="s">
+        <v>305</v>
+      </c>
+      <c r="N1" t="s">
         <v>306</v>
-      </c>
-      <c r="N1" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
@@ -23667,52 +23667,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="114"/>
-      <c r="B1" s="116"/>
-      <c r="C1" s="112" t="s">
+      <c r="A1" s="141"/>
+      <c r="B1" s="143"/>
+      <c r="C1" s="145" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
-      <c r="F1" s="112" t="s">
+      <c r="D1" s="145"/>
+      <c r="E1" s="145"/>
+      <c r="F1" s="145" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="112"/>
-      <c r="H1" s="112"/>
-      <c r="I1" s="112" t="s">
+      <c r="G1" s="145"/>
+      <c r="H1" s="145"/>
+      <c r="I1" s="145" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="112"/>
-      <c r="K1" s="112"/>
-      <c r="L1" s="112" t="s">
-        <v>300</v>
-      </c>
-      <c r="M1" s="112"/>
-      <c r="N1" s="112"/>
+      <c r="J1" s="145"/>
+      <c r="K1" s="145"/>
+      <c r="L1" s="145" t="s">
+        <v>299</v>
+      </c>
+      <c r="M1" s="145"/>
+      <c r="N1" s="145"/>
     </row>
     <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="115"/>
-      <c r="B2" s="117"/>
-      <c r="C2" s="113" t="s">
+      <c r="A2" s="142"/>
+      <c r="B2" s="144"/>
+      <c r="C2" s="146" t="s">
+        <v>447</v>
+      </c>
+      <c r="D2" s="146"/>
+      <c r="E2" s="146"/>
+      <c r="F2" s="146" t="s">
         <v>448</v>
       </c>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113" t="s">
+      <c r="G2" s="146"/>
+      <c r="H2" s="146"/>
+      <c r="I2" s="146" t="s">
         <v>449</v>
       </c>
-      <c r="G2" s="113"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="113" t="s">
+      <c r="J2" s="146"/>
+      <c r="K2" s="146"/>
+      <c r="L2" s="146" t="s">
         <v>450</v>
       </c>
-      <c r="J2" s="113"/>
-      <c r="K2" s="113"/>
-      <c r="L2" s="113" t="s">
-        <v>451</v>
-      </c>
-      <c r="M2" s="113"/>
-      <c r="N2" s="113"/>
+      <c r="M2" s="146"/>
+      <c r="N2" s="146"/>
     </row>
     <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="61" t="s">
@@ -23722,333 +23722,333 @@
         <v>2</v>
       </c>
       <c r="C3" s="63" t="s">
+        <v>300</v>
+      </c>
+      <c r="D3" s="63" t="s">
         <v>301</v>
       </c>
-      <c r="D3" s="63" t="s">
+      <c r="E3" s="63" t="s">
+        <v>389</v>
+      </c>
+      <c r="F3" s="62" t="s">
+        <v>300</v>
+      </c>
+      <c r="G3" s="63" t="s">
+        <v>301</v>
+      </c>
+      <c r="H3" s="63" t="s">
+        <v>389</v>
+      </c>
+      <c r="I3" s="62" t="s">
+        <v>300</v>
+      </c>
+      <c r="J3" s="63" t="s">
+        <v>301</v>
+      </c>
+      <c r="K3" s="63" t="s">
+        <v>389</v>
+      </c>
+      <c r="L3" s="62" t="s">
+        <v>300</v>
+      </c>
+      <c r="M3" s="63" t="s">
+        <v>301</v>
+      </c>
+      <c r="N3" s="63" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4" s="120" t="s">
+        <v>451</v>
+      </c>
+      <c r="B4" s="64" t="s">
         <v>302</v>
       </c>
-      <c r="E3" s="63" t="s">
-        <v>390</v>
-      </c>
-      <c r="F3" s="62" t="s">
-        <v>301</v>
-      </c>
-      <c r="G3" s="63" t="s">
-        <v>302</v>
-      </c>
-      <c r="H3" s="63" t="s">
-        <v>390</v>
-      </c>
-      <c r="I3" s="62" t="s">
-        <v>301</v>
-      </c>
-      <c r="J3" s="63" t="s">
-        <v>302</v>
-      </c>
-      <c r="K3" s="63" t="s">
-        <v>390</v>
-      </c>
-      <c r="L3" s="62" t="s">
-        <v>301</v>
-      </c>
-      <c r="M3" s="63" t="s">
-        <v>302</v>
-      </c>
-      <c r="N3" s="63" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="140" t="s">
-        <v>452</v>
-      </c>
-      <c r="B4" s="64" t="s">
-        <v>303</v>
-      </c>
       <c r="C4" s="65" t="s">
-        <v>372</v>
-      </c>
-      <c r="D4" s="122" t="s">
+        <v>371</v>
+      </c>
+      <c r="D4" s="140" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="120" t="s">
-        <v>374</v>
+      <c r="E4" s="139" t="s">
+        <v>373</v>
       </c>
       <c r="F4" s="65">
         <v>4.5</v>
       </c>
-      <c r="G4" s="122" t="s">
+      <c r="G4" s="140" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="120" t="s">
+      <c r="H4" s="139" t="s">
+        <v>303</v>
+      </c>
+      <c r="I4" s="65" t="s">
+        <v>374</v>
+      </c>
+      <c r="J4" s="140" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="139" t="s">
+        <v>376</v>
+      </c>
+      <c r="L4" s="84" t="s">
+        <v>377</v>
+      </c>
+      <c r="M4" s="138" t="s">
+        <v>7</v>
+      </c>
+      <c r="N4" s="139" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" s="119"/>
+      <c r="B5" s="70" t="s">
         <v>304</v>
       </c>
-      <c r="I4" s="65" t="s">
-        <v>375</v>
-      </c>
-      <c r="J4" s="122" t="s">
-        <v>7</v>
-      </c>
-      <c r="K4" s="120" t="s">
-        <v>377</v>
-      </c>
-      <c r="L4" s="84" t="s">
-        <v>378</v>
-      </c>
-      <c r="M4" s="118" t="s">
-        <v>7</v>
-      </c>
-      <c r="N4" s="120" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="139"/>
-      <c r="B5" s="70" t="s">
-        <v>305</v>
-      </c>
       <c r="C5" s="71" t="s">
-        <v>373</v>
-      </c>
-      <c r="D5" s="123"/>
-      <c r="E5" s="121"/>
+        <v>372</v>
+      </c>
+      <c r="D5" s="126"/>
+      <c r="E5" s="124"/>
       <c r="F5" s="71">
         <v>5.8</v>
       </c>
-      <c r="G5" s="123"/>
-      <c r="H5" s="121"/>
+      <c r="G5" s="126"/>
+      <c r="H5" s="124"/>
       <c r="I5" s="71" t="s">
-        <v>376</v>
-      </c>
-      <c r="J5" s="123"/>
-      <c r="K5" s="121"/>
+        <v>375</v>
+      </c>
+      <c r="J5" s="126"/>
+      <c r="K5" s="124"/>
       <c r="L5" s="76" t="s">
-        <v>379</v>
-      </c>
-      <c r="M5" s="119"/>
-      <c r="N5" s="121"/>
+        <v>378</v>
+      </c>
+      <c r="M5" s="128"/>
+      <c r="N5" s="124"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="138" t="s">
-        <v>453</v>
+      <c r="A6" s="118" t="s">
+        <v>452</v>
       </c>
       <c r="B6" s="78" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C6" s="79" t="s">
-        <v>363</v>
-      </c>
-      <c r="D6" s="133" t="s">
+        <v>362</v>
+      </c>
+      <c r="D6" s="125" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="134" t="s">
+      <c r="E6" s="123" t="s">
+        <v>364</v>
+      </c>
+      <c r="F6" s="80" t="s">
         <v>365</v>
       </c>
-      <c r="F6" s="80" t="s">
-        <v>366</v>
-      </c>
-      <c r="G6" s="137" t="s">
+      <c r="G6" s="127" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="135" t="s">
-        <v>368</v>
+      <c r="H6" s="121" t="s">
+        <v>367</v>
       </c>
       <c r="I6" s="79">
         <v>87</v>
       </c>
-      <c r="J6" s="133" t="s">
+      <c r="J6" s="125" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="135" t="s">
+      <c r="K6" s="121" t="s">
+        <v>367</v>
+      </c>
+      <c r="L6" s="79" t="s">
         <v>368</v>
       </c>
-      <c r="L6" s="79" t="s">
+      <c r="M6" s="125" t="s">
+        <v>13</v>
+      </c>
+      <c r="N6" s="121" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" s="119"/>
+      <c r="B7" s="70" t="s">
+        <v>304</v>
+      </c>
+      <c r="C7" s="71" t="s">
+        <v>363</v>
+      </c>
+      <c r="D7" s="126"/>
+      <c r="E7" s="124"/>
+      <c r="F7" s="76" t="s">
+        <v>366</v>
+      </c>
+      <c r="G7" s="128"/>
+      <c r="H7" s="122"/>
+      <c r="I7" s="71" t="s">
+        <v>342</v>
+      </c>
+      <c r="J7" s="126"/>
+      <c r="K7" s="122"/>
+      <c r="L7" s="71" t="s">
         <v>369</v>
       </c>
-      <c r="M6" s="133" t="s">
-        <v>13</v>
-      </c>
-      <c r="N6" s="135" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="139"/>
-      <c r="B7" s="70" t="s">
-        <v>305</v>
-      </c>
-      <c r="C7" s="71" t="s">
-        <v>364</v>
-      </c>
-      <c r="D7" s="123"/>
-      <c r="E7" s="121"/>
-      <c r="F7" s="76" t="s">
-        <v>367</v>
-      </c>
-      <c r="G7" s="119"/>
-      <c r="H7" s="125"/>
-      <c r="I7" s="71" t="s">
-        <v>343</v>
-      </c>
-      <c r="J7" s="123"/>
-      <c r="K7" s="125"/>
-      <c r="L7" s="71" t="s">
-        <v>370</v>
-      </c>
-      <c r="M7" s="123"/>
-      <c r="N7" s="125"/>
+      <c r="M7" s="126"/>
+      <c r="N7" s="122"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="138" t="s">
-        <v>454</v>
+      <c r="A8" s="118" t="s">
+        <v>453</v>
       </c>
       <c r="B8" s="78" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C8" s="79" t="s">
-        <v>356</v>
-      </c>
-      <c r="D8" s="133" t="s">
+        <v>355</v>
+      </c>
+      <c r="D8" s="125" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="134" t="s">
+      <c r="E8" s="123" t="s">
+        <v>357</v>
+      </c>
+      <c r="F8" s="80" t="s">
         <v>358</v>
       </c>
-      <c r="F8" s="80" t="s">
-        <v>359</v>
-      </c>
-      <c r="G8" s="137" t="s">
+      <c r="G8" s="127" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="135" t="s">
-        <v>361</v>
+      <c r="H8" s="121" t="s">
+        <v>360</v>
       </c>
       <c r="I8" s="79">
         <v>110</v>
       </c>
-      <c r="J8" s="133" t="s">
+      <c r="J8" s="125" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="135" t="s">
+      <c r="K8" s="121" t="s">
+        <v>360</v>
+      </c>
+      <c r="L8" s="79" t="s">
+        <v>308</v>
+      </c>
+      <c r="M8" s="125" t="s">
+        <v>13</v>
+      </c>
+      <c r="N8" s="121" t="s">
         <v>361</v>
       </c>
-      <c r="L8" s="79" t="s">
-        <v>309</v>
-      </c>
-      <c r="M8" s="133" t="s">
-        <v>13</v>
-      </c>
-      <c r="N8" s="135" t="s">
-        <v>362</v>
-      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="139"/>
+      <c r="A9" s="119"/>
       <c r="B9" s="70" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C9" s="71" t="s">
-        <v>357</v>
-      </c>
-      <c r="D9" s="123"/>
-      <c r="E9" s="121"/>
+        <v>356</v>
+      </c>
+      <c r="D9" s="126"/>
+      <c r="E9" s="124"/>
       <c r="F9" s="76" t="s">
-        <v>360</v>
-      </c>
-      <c r="G9" s="119"/>
-      <c r="H9" s="125"/>
+        <v>359</v>
+      </c>
+      <c r="G9" s="128"/>
+      <c r="H9" s="122"/>
       <c r="I9" s="71" t="s">
-        <v>344</v>
-      </c>
-      <c r="J9" s="123"/>
-      <c r="K9" s="125"/>
+        <v>343</v>
+      </c>
+      <c r="J9" s="126"/>
+      <c r="K9" s="122"/>
       <c r="L9" s="71" t="s">
-        <v>311</v>
-      </c>
-      <c r="M9" s="123"/>
-      <c r="N9" s="125"/>
+        <v>310</v>
+      </c>
+      <c r="M9" s="126"/>
+      <c r="N9" s="122"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="138" t="s">
+      <c r="A10" s="118" t="s">
+        <v>454</v>
+      </c>
+      <c r="B10" s="78" t="s">
+        <v>302</v>
+      </c>
+      <c r="C10" s="79" t="s">
+        <v>350</v>
+      </c>
+      <c r="D10" s="125" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="123" t="s">
+        <v>352</v>
+      </c>
+      <c r="F10" s="79" t="s">
+        <v>353</v>
+      </c>
+      <c r="G10" s="125" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="123" t="s">
+        <v>352</v>
+      </c>
+      <c r="I10" s="129">
+        <v>1.7</v>
+      </c>
+      <c r="J10" s="125" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10" s="123" t="s">
+        <v>352</v>
+      </c>
+      <c r="L10" s="129">
+        <v>3</v>
+      </c>
+      <c r="M10" s="125" t="s">
+        <v>7</v>
+      </c>
+      <c r="N10" s="123" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" s="119"/>
+      <c r="B11" s="70" t="s">
+        <v>304</v>
+      </c>
+      <c r="C11" s="71" t="s">
+        <v>351</v>
+      </c>
+      <c r="D11" s="126"/>
+      <c r="E11" s="124"/>
+      <c r="F11" s="71" t="s">
+        <v>354</v>
+      </c>
+      <c r="G11" s="126"/>
+      <c r="H11" s="124"/>
+      <c r="I11" s="130"/>
+      <c r="J11" s="126"/>
+      <c r="K11" s="124"/>
+      <c r="L11" s="130"/>
+      <c r="M11" s="126"/>
+      <c r="N11" s="124"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" s="118" t="s">
         <v>455</v>
       </c>
-      <c r="B10" s="78" t="s">
-        <v>303</v>
-      </c>
-      <c r="C10" s="79" t="s">
-        <v>351</v>
-      </c>
-      <c r="D10" s="133" t="s">
+      <c r="B12" s="78" t="s">
+        <v>302</v>
+      </c>
+      <c r="C12" s="79" t="s">
+        <v>345</v>
+      </c>
+      <c r="D12" s="125" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="134" t="s">
-        <v>353</v>
-      </c>
-      <c r="F10" s="79" t="s">
-        <v>354</v>
-      </c>
-      <c r="G10" s="133" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" s="134" t="s">
-        <v>353</v>
-      </c>
-      <c r="I10" s="136">
-        <v>1.7</v>
-      </c>
-      <c r="J10" s="133" t="s">
-        <v>7</v>
-      </c>
-      <c r="K10" s="134" t="s">
-        <v>353</v>
-      </c>
-      <c r="L10" s="136">
-        <v>3</v>
-      </c>
-      <c r="M10" s="133" t="s">
-        <v>7</v>
-      </c>
-      <c r="N10" s="134" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="139"/>
-      <c r="B11" s="70" t="s">
-        <v>305</v>
-      </c>
-      <c r="C11" s="71" t="s">
-        <v>352</v>
-      </c>
-      <c r="D11" s="123"/>
-      <c r="E11" s="121"/>
-      <c r="F11" s="71" t="s">
-        <v>355</v>
-      </c>
-      <c r="G11" s="123"/>
-      <c r="H11" s="121"/>
-      <c r="I11" s="128"/>
-      <c r="J11" s="123"/>
-      <c r="K11" s="121"/>
-      <c r="L11" s="128"/>
-      <c r="M11" s="123"/>
-      <c r="N11" s="121"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="138" t="s">
-        <v>456</v>
-      </c>
-      <c r="B12" s="78" t="s">
-        <v>303</v>
-      </c>
-      <c r="C12" s="79" t="s">
-        <v>346</v>
-      </c>
-      <c r="D12" s="133" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="134" t="s">
-        <v>348</v>
+      <c r="E12" s="123" t="s">
+        <v>347</v>
       </c>
       <c r="F12" s="80"/>
       <c r="G12" s="78"/>
@@ -24056,59 +24056,59 @@
       <c r="I12" s="79">
         <v>2.4</v>
       </c>
-      <c r="J12" s="133" t="s">
+      <c r="J12" s="125" t="s">
         <v>26</v>
       </c>
-      <c r="K12" s="134" t="s">
+      <c r="K12" s="123" t="s">
+        <v>348</v>
+      </c>
+      <c r="L12" s="129">
+        <v>32</v>
+      </c>
+      <c r="M12" s="125" t="s">
+        <v>7</v>
+      </c>
+      <c r="N12" s="121" t="s">
         <v>349</v>
       </c>
-      <c r="L12" s="136">
-        <v>32</v>
-      </c>
-      <c r="M12" s="133" t="s">
-        <v>7</v>
-      </c>
-      <c r="N12" s="135" t="s">
-        <v>350</v>
-      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="139"/>
+      <c r="A13" s="119"/>
       <c r="B13" s="70" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C13" s="71" t="s">
-        <v>347</v>
-      </c>
-      <c r="D13" s="123"/>
-      <c r="E13" s="121"/>
+        <v>346</v>
+      </c>
+      <c r="D13" s="126"/>
+      <c r="E13" s="124"/>
       <c r="F13" s="76"/>
       <c r="G13" s="70"/>
       <c r="H13" s="75"/>
       <c r="I13" s="71">
         <v>5.3</v>
       </c>
-      <c r="J13" s="123"/>
-      <c r="K13" s="121"/>
-      <c r="L13" s="128"/>
-      <c r="M13" s="123"/>
-      <c r="N13" s="125"/>
+      <c r="J13" s="126"/>
+      <c r="K13" s="124"/>
+      <c r="L13" s="130"/>
+      <c r="M13" s="126"/>
+      <c r="N13" s="122"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" s="138" t="s">
-        <v>457</v>
+      <c r="A14" s="118" t="s">
+        <v>456</v>
       </c>
       <c r="B14" s="78" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C14" s="79" t="s">
-        <v>340</v>
-      </c>
-      <c r="D14" s="133" t="s">
+        <v>339</v>
+      </c>
+      <c r="D14" s="125" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="134" t="s">
-        <v>342</v>
+      <c r="E14" s="123" t="s">
+        <v>341</v>
       </c>
       <c r="F14" s="79"/>
       <c r="G14" s="82"/>
@@ -24117,25 +24117,25 @@
       <c r="J14" s="82"/>
       <c r="K14" s="83"/>
       <c r="L14" s="79" t="s">
-        <v>343</v>
-      </c>
-      <c r="M14" s="133" t="s">
+        <v>342</v>
+      </c>
+      <c r="M14" s="125" t="s">
         <v>7</v>
       </c>
-      <c r="N14" s="135" t="s">
-        <v>345</v>
+      <c r="N14" s="121" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="139"/>
+      <c r="A15" s="119"/>
       <c r="B15" s="70" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C15" s="71" t="s">
-        <v>341</v>
-      </c>
-      <c r="D15" s="123"/>
-      <c r="E15" s="121"/>
+        <v>340</v>
+      </c>
+      <c r="D15" s="126"/>
+      <c r="E15" s="124"/>
       <c r="F15" s="71"/>
       <c r="G15" s="72"/>
       <c r="H15" s="77"/>
@@ -24143,158 +24143,158 @@
       <c r="J15" s="72"/>
       <c r="K15" s="77"/>
       <c r="L15" s="71" t="s">
-        <v>344</v>
-      </c>
-      <c r="M15" s="123"/>
-      <c r="N15" s="125"/>
+        <v>343</v>
+      </c>
+      <c r="M15" s="126"/>
+      <c r="N15" s="122"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="138" t="s">
-        <v>458</v>
+      <c r="A16" s="118" t="s">
+        <v>457</v>
       </c>
       <c r="B16" s="66" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C16" s="67" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D16" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="132" t="s">
-        <v>391</v>
+      <c r="E16" s="133" t="s">
+        <v>390</v>
       </c>
       <c r="F16" s="67">
         <v>16</v>
       </c>
-      <c r="G16" s="129" t="s">
+      <c r="G16" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="H16" s="124" t="s">
-        <v>335</v>
+      <c r="H16" s="132" t="s">
+        <v>334</v>
       </c>
       <c r="I16" s="68" t="s">
+        <v>336</v>
+      </c>
+      <c r="J16" s="131" t="s">
+        <v>7</v>
+      </c>
+      <c r="K16" s="133" t="s">
         <v>337</v>
       </c>
-      <c r="J16" s="126" t="s">
-        <v>7</v>
-      </c>
-      <c r="K16" s="132" t="s">
+      <c r="L16" s="135" t="s">
         <v>338</v>
       </c>
-      <c r="L16" s="127" t="s">
-        <v>339</v>
-      </c>
-      <c r="M16" s="126" t="s">
+      <c r="M16" s="131" t="s">
         <v>13</v>
       </c>
-      <c r="N16" s="124" t="s">
-        <v>392</v>
+      <c r="N16" s="132" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A17" s="139"/>
+      <c r="A17" s="119"/>
       <c r="B17" s="70" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C17" s="71" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D17" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="121"/>
+      <c r="E17" s="124"/>
       <c r="F17" s="71">
         <v>22</v>
       </c>
-      <c r="G17" s="119"/>
-      <c r="H17" s="125"/>
+      <c r="G17" s="128"/>
+      <c r="H17" s="122"/>
       <c r="I17" s="76" t="s">
-        <v>336</v>
-      </c>
-      <c r="J17" s="123"/>
-      <c r="K17" s="121"/>
-      <c r="L17" s="128"/>
-      <c r="M17" s="123"/>
-      <c r="N17" s="125"/>
+        <v>335</v>
+      </c>
+      <c r="J17" s="126"/>
+      <c r="K17" s="124"/>
+      <c r="L17" s="130"/>
+      <c r="M17" s="126"/>
+      <c r="N17" s="122"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A18" s="138" t="s">
-        <v>459</v>
+      <c r="A18" s="118" t="s">
+        <v>458</v>
       </c>
       <c r="B18" s="66" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C18" s="67" t="s">
-        <v>325</v>
-      </c>
-      <c r="D18" s="126" t="s">
+        <v>324</v>
+      </c>
+      <c r="D18" s="131" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="132" t="s">
+      <c r="E18" s="133" t="s">
+        <v>326</v>
+      </c>
+      <c r="F18" s="68" t="s">
         <v>327</v>
       </c>
-      <c r="F18" s="68" t="s">
-        <v>328</v>
-      </c>
-      <c r="G18" s="129" t="s">
+      <c r="G18" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="H18" s="124" t="s">
-        <v>330</v>
+      <c r="H18" s="132" t="s">
+        <v>329</v>
       </c>
       <c r="I18" s="67"/>
       <c r="J18" s="69"/>
       <c r="K18" s="73"/>
       <c r="L18" s="67" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="M18" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="N18" s="124" t="s">
-        <v>321</v>
+      <c r="N18" s="132" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A19" s="139"/>
+      <c r="A19" s="119"/>
       <c r="B19" s="70" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C19" s="71" t="s">
-        <v>326</v>
-      </c>
-      <c r="D19" s="123"/>
-      <c r="E19" s="121"/>
+        <v>325</v>
+      </c>
+      <c r="D19" s="126"/>
+      <c r="E19" s="124"/>
       <c r="F19" s="76" t="s">
-        <v>329</v>
-      </c>
-      <c r="G19" s="119"/>
-      <c r="H19" s="125"/>
+        <v>328</v>
+      </c>
+      <c r="G19" s="128"/>
+      <c r="H19" s="122"/>
       <c r="I19" s="71"/>
       <c r="J19" s="72"/>
       <c r="K19" s="77"/>
       <c r="L19" s="71" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="M19" s="72"/>
-      <c r="N19" s="125"/>
+      <c r="N19" s="122"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A20" s="138" t="s">
-        <v>460</v>
+      <c r="A20" s="118" t="s">
+        <v>459</v>
       </c>
       <c r="B20" s="66" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C20" s="67" t="s">
-        <v>322</v>
-      </c>
-      <c r="D20" s="126" t="s">
+        <v>321</v>
+      </c>
+      <c r="D20" s="131" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="132" t="s">
-        <v>324</v>
+      <c r="E20" s="133" t="s">
+        <v>323</v>
       </c>
       <c r="F20" s="68"/>
       <c r="G20" s="66"/>
@@ -24303,25 +24303,25 @@
       <c r="J20" s="66"/>
       <c r="K20" s="74"/>
       <c r="L20" s="68" t="s">
-        <v>319</v>
-      </c>
-      <c r="M20" s="126" t="s">
+        <v>318</v>
+      </c>
+      <c r="M20" s="131" t="s">
         <v>13</v>
       </c>
-      <c r="N20" s="124" t="s">
-        <v>321</v>
+      <c r="N20" s="132" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A21" s="139"/>
+      <c r="A21" s="119"/>
       <c r="B21" s="70" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C21" s="71" t="s">
-        <v>323</v>
-      </c>
-      <c r="D21" s="123"/>
-      <c r="E21" s="121"/>
+        <v>322</v>
+      </c>
+      <c r="D21" s="126"/>
+      <c r="E21" s="124"/>
       <c r="F21" s="76"/>
       <c r="G21" s="70"/>
       <c r="H21" s="75"/>
@@ -24329,17 +24329,17 @@
       <c r="J21" s="70"/>
       <c r="K21" s="75"/>
       <c r="L21" s="76" t="s">
-        <v>320</v>
-      </c>
-      <c r="M21" s="123"/>
-      <c r="N21" s="125"/>
+        <v>319</v>
+      </c>
+      <c r="M21" s="126"/>
+      <c r="N21" s="122"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A22" s="138" t="s">
-        <v>461</v>
+      <c r="A22" s="118" t="s">
+        <v>460</v>
       </c>
       <c r="B22" s="66" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C22" s="68"/>
       <c r="D22" s="66"/>
@@ -24350,20 +24350,20 @@
       <c r="I22" s="68"/>
       <c r="J22" s="66"/>
       <c r="K22" s="74"/>
-      <c r="L22" s="130" t="s">
-        <v>316</v>
-      </c>
-      <c r="M22" s="126" t="s">
+      <c r="L22" s="136" t="s">
+        <v>315</v>
+      </c>
+      <c r="M22" s="131" t="s">
         <v>13</v>
       </c>
-      <c r="N22" s="124" t="s">
-        <v>308</v>
+      <c r="N22" s="132" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A23" s="139"/>
+      <c r="A23" s="119"/>
       <c r="B23" s="70" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C23" s="76"/>
       <c r="D23" s="70"/>
@@ -24374,108 +24374,131 @@
       <c r="I23" s="76"/>
       <c r="J23" s="70"/>
       <c r="K23" s="75"/>
-      <c r="L23" s="131"/>
-      <c r="M23" s="123"/>
-      <c r="N23" s="125"/>
+      <c r="L23" s="137"/>
+      <c r="M23" s="126"/>
+      <c r="N23" s="122"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A24" s="138" t="s">
-        <v>462</v>
+      <c r="A24" s="118" t="s">
+        <v>461</v>
       </c>
       <c r="B24" s="66" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C24" s="68" t="s">
-        <v>314</v>
-      </c>
-      <c r="D24" s="126" t="s">
+        <v>313</v>
+      </c>
+      <c r="D24" s="131" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="132" t="s">
-        <v>317</v>
+      <c r="E24" s="133" t="s">
+        <v>316</v>
       </c>
       <c r="F24" s="67" t="s">
-        <v>312</v>
-      </c>
-      <c r="G24" s="129" t="s">
+        <v>311</v>
+      </c>
+      <c r="G24" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="H24" s="132" t="s">
-        <v>317</v>
+      <c r="H24" s="133" t="s">
+        <v>316</v>
       </c>
       <c r="I24" s="68">
         <v>3.3</v>
       </c>
-      <c r="J24" s="129" t="s">
+      <c r="J24" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="K24" s="132" t="s">
+      <c r="K24" s="133" t="s">
+        <v>316</v>
+      </c>
+      <c r="L24" s="135" t="s">
+        <v>308</v>
+      </c>
+      <c r="M24" s="131" t="s">
+        <v>7</v>
+      </c>
+      <c r="N24" s="132" t="s">
         <v>317</v>
       </c>
-      <c r="L24" s="127" t="s">
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A25" s="119"/>
+      <c r="B25" s="70" t="s">
+        <v>304</v>
+      </c>
+      <c r="C25" s="76" t="s">
+        <v>314</v>
+      </c>
+      <c r="D25" s="126"/>
+      <c r="E25" s="124"/>
+      <c r="F25" s="71" t="s">
+        <v>312</v>
+      </c>
+      <c r="G25" s="128"/>
+      <c r="H25" s="124"/>
+      <c r="I25" s="76" t="s">
         <v>309</v>
       </c>
-      <c r="M24" s="126" t="s">
-        <v>7</v>
-      </c>
-      <c r="N24" s="124" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A25" s="139"/>
-      <c r="B25" s="70" t="s">
-        <v>305</v>
-      </c>
-      <c r="C25" s="76" t="s">
-        <v>315</v>
-      </c>
-      <c r="D25" s="123"/>
-      <c r="E25" s="121"/>
-      <c r="F25" s="71" t="s">
-        <v>313</v>
-      </c>
-      <c r="G25" s="119"/>
-      <c r="H25" s="121"/>
-      <c r="I25" s="76" t="s">
-        <v>310</v>
-      </c>
-      <c r="J25" s="119"/>
-      <c r="K25" s="121"/>
-      <c r="L25" s="128"/>
-      <c r="M25" s="123"/>
-      <c r="N25" s="125"/>
+      <c r="J25" s="128"/>
+      <c r="K25" s="124"/>
+      <c r="L25" s="130"/>
+      <c r="M25" s="126"/>
+      <c r="N25" s="122"/>
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="N20:N21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="N24:N25"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="M14:M15"/>
     <mergeCell ref="N12:N13"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:E11"/>
@@ -24492,57 +24515,34 @@
     <mergeCell ref="K12:K13"/>
     <mergeCell ref="L12:L13"/>
     <mergeCell ref="M12:M13"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="N20:N21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="N24:N25"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="M20:M21"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -30944,41 +30944,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="143" t="s">
-        <v>407</v>
-      </c>
-      <c r="B1" s="143"/>
-      <c r="C1" s="143"/>
-      <c r="D1" s="143"/>
-      <c r="E1" s="143"/>
-      <c r="F1" s="143"/>
+      <c r="A1" s="149" t="s">
+        <v>406</v>
+      </c>
+      <c r="B1" s="149"/>
+      <c r="C1" s="149"/>
+      <c r="D1" s="149"/>
+      <c r="E1" s="149"/>
+      <c r="F1" s="149"/>
     </row>
     <row r="2" spans="1:10" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="91" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B2" s="91" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C2" s="91" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D2" s="91" t="s">
+        <v>394</v>
+      </c>
+      <c r="E2" s="91" t="s">
         <v>395</v>
       </c>
-      <c r="E2" s="91" t="s">
+      <c r="F2" s="91" t="s">
         <v>396</v>
-      </c>
-      <c r="F2" s="91" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="27" x14ac:dyDescent="0.35">
       <c r="A3" s="92" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B3" s="93" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C3" s="93">
         <v>45.45</v>
@@ -30994,13 +30994,13 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="145" t="s">
+      <c r="A4" s="151" t="s">
+        <v>398</v>
+      </c>
+      <c r="B4" s="95" t="s">
         <v>399</v>
       </c>
-      <c r="B4" s="95" t="s">
-        <v>400</v>
-      </c>
-      <c r="C4" s="147">
+      <c r="C4" s="153">
         <v>100</v>
       </c>
       <c r="D4" s="95">
@@ -31014,11 +31014,11 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="145"/>
+      <c r="A5" s="151"/>
       <c r="B5" s="96" t="s">
-        <v>401</v>
-      </c>
-      <c r="C5" s="145"/>
+        <v>400</v>
+      </c>
+      <c r="C5" s="151"/>
       <c r="D5" s="96">
         <v>-2.0699999999999998</v>
       </c>
@@ -31030,11 +31030,11 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="145"/>
+      <c r="A6" s="151"/>
       <c r="B6" s="97" t="s">
-        <v>447</v>
-      </c>
-      <c r="C6" s="145"/>
+        <v>446</v>
+      </c>
+      <c r="C6" s="151"/>
       <c r="D6" s="96">
         <v>4.16</v>
       </c>
@@ -31046,11 +31046,11 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="145"/>
+      <c r="A7" s="151"/>
       <c r="B7" s="97" t="s">
-        <v>446</v>
-      </c>
-      <c r="C7" s="145"/>
+        <v>445</v>
+      </c>
+      <c r="C7" s="151"/>
       <c r="D7" s="96">
         <v>3.11</v>
       </c>
@@ -31062,11 +31062,11 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="25" x14ac:dyDescent="0.35">
-      <c r="A8" s="145"/>
+      <c r="A8" s="151"/>
       <c r="B8" s="96" t="s">
-        <v>472</v>
-      </c>
-      <c r="C8" s="145"/>
+        <v>471</v>
+      </c>
+      <c r="C8" s="151"/>
       <c r="D8" s="96">
         <v>-2.68</v>
       </c>
@@ -31078,13 +31078,13 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="146"/>
+      <c r="A9" s="152"/>
       <c r="B9" s="93" t="s">
+        <v>401</v>
+      </c>
+      <c r="C9" s="152"/>
+      <c r="D9" s="93" t="s">
         <v>402</v>
-      </c>
-      <c r="C9" s="146"/>
-      <c r="D9" s="93" t="s">
-        <v>403</v>
       </c>
       <c r="E9" s="93">
         <v>0</v>
@@ -31094,80 +31094,80 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="148" t="s">
+      <c r="A10" s="154" t="s">
+        <v>407</v>
+      </c>
+      <c r="B10" s="98" t="s">
+        <v>409</v>
+      </c>
+      <c r="C10" s="153">
+        <v>100</v>
+      </c>
+      <c r="D10" s="98" t="s">
+        <v>403</v>
+      </c>
+      <c r="E10" s="153">
+        <v>0</v>
+      </c>
+      <c r="F10" s="153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="154"/>
+      <c r="B11" s="98" t="s">
         <v>408</v>
       </c>
-      <c r="B10" s="98" t="s">
+      <c r="C11" s="154"/>
+      <c r="D11" s="98" t="s">
+        <v>404</v>
+      </c>
+      <c r="E11" s="154"/>
+      <c r="F11" s="154"/>
+    </row>
+    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="155"/>
+      <c r="B12" s="99" t="s">
         <v>410</v>
       </c>
-      <c r="C10" s="147">
-        <v>100</v>
-      </c>
-      <c r="D10" s="98" t="s">
-        <v>404</v>
-      </c>
-      <c r="E10" s="147">
-        <v>0</v>
-      </c>
-      <c r="F10" s="147">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="148"/>
-      <c r="B11" s="98" t="s">
-        <v>409</v>
-      </c>
-      <c r="C11" s="148"/>
-      <c r="D11" s="98" t="s">
+      <c r="C12" s="155"/>
+      <c r="D12" s="99" t="s">
         <v>405</v>
       </c>
-      <c r="E11" s="148"/>
-      <c r="F11" s="148"/>
-    </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="149"/>
-      <c r="B12" s="99" t="s">
+      <c r="E12" s="155"/>
+      <c r="F12" s="155"/>
+    </row>
+    <row r="13" spans="1:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="149" t="s">
         <v>411</v>
       </c>
-      <c r="C12" s="149"/>
-      <c r="D12" s="99" t="s">
-        <v>406</v>
-      </c>
-      <c r="E12" s="149"/>
-      <c r="F12" s="149"/>
-    </row>
-    <row r="13" spans="1:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="143" t="s">
-        <v>412</v>
-      </c>
-      <c r="B13" s="143"/>
-      <c r="C13" s="143"/>
-      <c r="D13" s="143"/>
-      <c r="E13" s="143"/>
-      <c r="F13" s="143"/>
+      <c r="B13" s="149"/>
+      <c r="C13" s="149"/>
+      <c r="D13" s="149"/>
+      <c r="E13" s="149"/>
+      <c r="F13" s="149"/>
     </row>
     <row r="14" spans="1:10" ht="95" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="100" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="100" t="s">
+        <v>416</v>
+      </c>
+      <c r="C14" s="101" t="s">
+        <v>462</v>
+      </c>
+      <c r="D14" s="102" t="s">
+        <v>415</v>
+      </c>
+      <c r="E14" s="91" t="s">
+        <v>469</v>
+      </c>
+      <c r="F14" s="91" t="s">
+        <v>470</v>
+      </c>
+      <c r="H14" s="59" t="s">
         <v>417</v>
-      </c>
-      <c r="C14" s="101" t="s">
-        <v>463</v>
-      </c>
-      <c r="D14" s="102" t="s">
-        <v>416</v>
-      </c>
-      <c r="E14" s="91" t="s">
-        <v>470</v>
-      </c>
-      <c r="F14" s="91" t="s">
-        <v>471</v>
-      </c>
-      <c r="H14" s="59" t="s">
-        <v>418</v>
       </c>
       <c r="I14" s="59"/>
       <c r="J14" s="85"/>
@@ -31269,38 +31269,38 @@
       <c r="I18" s="87"/>
     </row>
     <row r="19" spans="1:9" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="144" t="s">
-        <v>413</v>
-      </c>
-      <c r="B19" s="144"/>
-      <c r="C19" s="144"/>
-      <c r="D19" s="144"/>
-      <c r="E19" s="144"/>
-      <c r="F19" s="144"/>
+      <c r="A19" s="150" t="s">
+        <v>412</v>
+      </c>
+      <c r="B19" s="150"/>
+      <c r="C19" s="150"/>
+      <c r="D19" s="150"/>
+      <c r="E19" s="150"/>
+      <c r="F19" s="150"/>
     </row>
     <row r="20" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="106" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="142" t="s">
-        <v>414</v>
-      </c>
-      <c r="C20" s="142"/>
-      <c r="D20" s="142"/>
-      <c r="E20" s="142"/>
+      <c r="B20" s="148" t="s">
+        <v>413</v>
+      </c>
+      <c r="C20" s="148"/>
+      <c r="D20" s="148"/>
+      <c r="E20" s="148"/>
       <c r="F20" s="107"/>
     </row>
     <row r="21" spans="1:9" ht="16.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="100" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="141" t="s">
-        <v>415</v>
-      </c>
-      <c r="C21" s="141"/>
-      <c r="D21" s="141"/>
-      <c r="E21" s="141"/>
-      <c r="F21" s="141"/>
+      <c r="B21" s="147" t="s">
+        <v>414</v>
+      </c>
+      <c r="C21" s="147"/>
+      <c r="D21" s="147"/>
+      <c r="E21" s="147"/>
+      <c r="F21" s="147"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -31338,18 +31338,18 @@
   <sheetData>
     <row r="1" spans="1:12" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="89" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B1" s="90" t="s">
+        <v>419</v>
+      </c>
+      <c r="C1" s="90" t="s">
         <v>420</v>
-      </c>
-      <c r="C1" s="90" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="55" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B2" s="108">
         <v>9.4855999999999998</v>
@@ -31358,15 +31358,15 @@
         <v>100</v>
       </c>
       <c r="G2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="55" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B3" s="108">
         <v>7.0216000000000003</v>
@@ -31375,7 +31375,7 @@
         <v>73.251000000000005</v>
       </c>
       <c r="F3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="G3" s="12">
         <v>9.4855999999999998</v>
@@ -31384,12 +31384,12 @@
         <v>100</v>
       </c>
       <c r="K3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="56" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B4" s="108">
         <v>6.3212000000000002</v>
@@ -31398,7 +31398,7 @@
         <v>65.647000000000006</v>
       </c>
       <c r="F4" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="G4" s="12">
         <v>7.0216000000000003</v>
@@ -31407,12 +31407,12 @@
         <v>73.251000000000005</v>
       </c>
       <c r="K4" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="55" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B5" s="108">
         <v>6.1144999999999996</v>
@@ -31435,7 +31435,7 @@
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="55" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B6" s="108">
         <v>4.8567</v>
@@ -31458,7 +31458,7 @@
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="55" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B7" s="108">
         <v>4.3666</v>
@@ -31481,7 +31481,7 @@
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="88" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B8" s="108">
         <v>4.1395999999999997</v>
@@ -31504,7 +31504,7 @@
     </row>
     <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="55" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B9" s="108">
         <v>3.7168999999999999</v>
@@ -31513,7 +31513,7 @@
         <v>37.375</v>
       </c>
       <c r="F9" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="G9" s="12">
         <v>4.1395999999999997</v>
@@ -31522,12 +31522,12 @@
         <v>41.963000000000001</v>
       </c>
       <c r="K9" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="55" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B10" s="108">
         <v>3.2614000000000001</v>
@@ -31550,7 +31550,7 @@
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="56" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B11" s="108">
         <v>3.1615000000000002</v>
@@ -31573,7 +31573,7 @@
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="55" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B12" s="108">
         <v>2.5590000000000002</v>
@@ -31619,7 +31619,7 @@
     </row>
     <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="56" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B14" s="108">
         <v>1.9306000000000001</v>
@@ -31642,7 +31642,7 @@
     </row>
     <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="56" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B15" s="108">
         <v>0.60829999999999995</v>
@@ -31665,7 +31665,7 @@
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="57" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B16" s="109">
         <v>0.27429999999999999</v>
@@ -31709,62 +31709,62 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="55" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="55" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="55" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="55" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="55" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="56" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="55" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="55" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="56" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="55" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="56" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="55" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
@@ -31774,17 +31774,17 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="56" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="56" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="57" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>